<commit_message>
elder job started after adding related excel file
</commit_message>
<xml_diff>
--- a/iwasa_paper_02_severn.xlsx
+++ b/iwasa_paper_02_severn.xlsx
@@ -421,9 +421,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>St1 @ 2.1 (km)</t>
-  </si>
-  <si>
     <t>St2 @ 1.175 (km)</t>
   </si>
   <si>
@@ -446,6 +443,9 @@
   </si>
   <si>
     <t>Observed Concentration [ppm] using formula2</t>
+  </si>
+  <si>
+    <t>St1 @ 0.21 (km)</t>
   </si>
 </sst>
 </file>
@@ -4679,8 +4679,8 @@
   </sheetPr>
   <dimension ref="A1:X91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4958,7 +4958,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="53">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -7081,9 +7081,9 @@
   </sheetPr>
   <dimension ref="A1:AP21"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7249,15 +7249,15 @@
         <v>82</v>
       </c>
       <c r="AO1" s="104" t="s">
+        <v>111</v>
+      </c>
+      <c r="AP1" s="104" t="s">
         <v>112</v>
-      </c>
-      <c r="AP1" s="104" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:42" s="80" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="75" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B2" s="76">
         <v>0</v>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="AB2" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AC2" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7353,7 +7353,7 @@
       </c>
       <c r="AE2" s="80">
         <f t="shared" ref="AE2:AE3" si="0">Delta_T__seconds</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AF2" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7400,7 +7400,7 @@
     </row>
     <row r="3" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="76">
         <f>C2</f>
@@ -7485,7 +7485,7 @@
       </c>
       <c r="AB3" s="82">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="AC3" s="82">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7497,7 +7497,7 @@
       </c>
       <c r="AE3" s="80">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AF3" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7544,7 +7544,7 @@
     </row>
     <row r="4" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="76">
         <f t="shared" ref="B4:B8" si="2">C3</f>
@@ -7629,7 +7629,7 @@
       </c>
       <c r="AB4" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="AC4" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7641,7 +7641,7 @@
       </c>
       <c r="AE4" s="80">
         <f>Delta_T__seconds</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AF4" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7684,7 +7684,7 @@
     </row>
     <row r="5" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="85" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="76">
         <f t="shared" si="2"/>
@@ -7769,7 +7769,7 @@
       </c>
       <c r="AB5" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>253</v>
+        <v>355</v>
       </c>
       <c r="AC5" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7781,7 +7781,7 @@
       </c>
       <c r="AE5" s="80">
         <f>Delta_T__seconds</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AF5" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7824,7 +7824,7 @@
     </row>
     <row r="6" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="76">
         <f t="shared" si="2"/>
@@ -7909,7 +7909,7 @@
       </c>
       <c r="AB6" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>383</v>
+        <v>537</v>
       </c>
       <c r="AC6" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -7921,7 +7921,7 @@
       </c>
       <c r="AE6" s="80">
         <f>Delta_T__seconds</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AF6" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -7964,7 +7964,7 @@
     </row>
     <row r="7" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="85" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="76">
         <f t="shared" si="2"/>
@@ -8049,7 +8049,7 @@
       </c>
       <c r="AB7" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>517</v>
+        <v>724</v>
       </c>
       <c r="AC7" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -8061,7 +8061,7 @@
       </c>
       <c r="AE7" s="80">
         <f>Delta_T__seconds</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AF7" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8104,7 +8104,7 @@
     </row>
     <row r="8" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="76">
         <f t="shared" si="2"/>
@@ -8189,7 +8189,7 @@
       </c>
       <c r="AB8" s="89">
         <f>FLOOR((Table1[[#This Row],[Tp]]*3600)/Table1[[#This Row],[Delta T]],1)</f>
-        <v>672</v>
+        <v>941</v>
       </c>
       <c r="AC8" s="89">
         <f>Table1[[#This Row],[End Point distance  '[meters']]]/Delta_X__meters</f>
@@ -8201,7 +8201,7 @@
       </c>
       <c r="AE8" s="80">
         <f>Delta_T__seconds</f>
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="AF8" s="81">
         <f>((Table1[[#This Row],[Ti]]-Table1[[#This Row],[calculated time '[hours']]])/Table1[[#This Row],[Ti]])</f>
@@ -8259,9 +8259,6 @@
       <c r="Z15" s="94"/>
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="D16" s="67">
-        <v>18000</v>
-      </c>
       <c r="Y16" s="99"/>
       <c r="Z16" s="95"/>
     </row>

</xml_diff>